<commit_message>
Incorporate TopSky 2.3 and add ICAO datafiles
- Fixes #31
- Adds ICAO Datafiles in pack
</commit_message>
<xml_diff>
--- a/UK-TopSky/Data/Plugin/TopSky/TopSky_Developer_Guide_Settings.xlsx
+++ b/UK-TopSky/Data/Plugin/TopSky/TopSky_Developer_Guide_Settings.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juha\Documents\Office Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A072E26-689E-4794-83B1-D14985265903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C286C04B-512D-4126-BC62-AB3FA033D8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="210" windowWidth="28530" windowHeight="16350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TopSky 2.3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -5914,8 +5912,8 @@
   <dimension ref="A1:M743"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A261" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A267" sqref="A267"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19393,6 +19391,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -19979,28 +19978,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>